<commit_message>
main correction and comment
commented section of code and corrected to main to check position
</commit_message>
<xml_diff>
--- a/sun data/SunData.xlsx
+++ b/sun data/SunData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rbake\PycharmProjects\Sun track-in\Sun Track-in\sun data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EAF22AD-00E7-43C4-B467-15638F759AA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AC2F466-FF96-4B01-A947-A8904C4FBCA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2664" yWindow="2700" windowWidth="17280" windowHeight="8964" xr2:uid="{D8B1F0AE-B319-452F-A3FC-826487B52C7D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D8B1F0AE-B319-452F-A3FC-826487B52C7D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0B8B9FF-2C04-4644-8C06-A3DF4BC84741}">
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:C53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -823,6 +823,171 @@
         <v>2.4700000000000002</v>
       </c>
     </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>1630</v>
+      </c>
+      <c r="B39">
+        <v>237.6</v>
+      </c>
+      <c r="C39">
+        <v>2.4700000000000002</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>1645</v>
+      </c>
+      <c r="B40">
+        <v>237.6</v>
+      </c>
+      <c r="C40">
+        <v>2.4700000000000002</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>1700</v>
+      </c>
+      <c r="B41">
+        <v>237.6</v>
+      </c>
+      <c r="C41">
+        <v>2.4700000000000002</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>1715</v>
+      </c>
+      <c r="B42">
+        <v>237.6</v>
+      </c>
+      <c r="C42">
+        <v>2.4700000000000002</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>1730</v>
+      </c>
+      <c r="B43">
+        <v>237.6</v>
+      </c>
+      <c r="C43">
+        <v>2.4700000000000002</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>1745</v>
+      </c>
+      <c r="B44">
+        <v>237.6</v>
+      </c>
+      <c r="C44">
+        <v>2.4700000000000002</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>1800</v>
+      </c>
+      <c r="B45">
+        <v>237.6</v>
+      </c>
+      <c r="C45">
+        <v>2.4700000000000002</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>1815</v>
+      </c>
+      <c r="B46">
+        <v>237.6</v>
+      </c>
+      <c r="C46">
+        <v>2.4700000000000002</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>1830</v>
+      </c>
+      <c r="B47">
+        <v>237.6</v>
+      </c>
+      <c r="C47">
+        <v>2.4700000000000002</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>1845</v>
+      </c>
+      <c r="B48">
+        <v>237.6</v>
+      </c>
+      <c r="C48">
+        <v>2.4700000000000002</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>1900</v>
+      </c>
+      <c r="B49">
+        <v>237.6</v>
+      </c>
+      <c r="C49">
+        <v>2.4700000000000002</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>1915</v>
+      </c>
+      <c r="B50">
+        <v>237.6</v>
+      </c>
+      <c r="C50">
+        <v>2.4700000000000002</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>1930</v>
+      </c>
+      <c r="B51">
+        <v>237.6</v>
+      </c>
+      <c r="C51">
+        <v>2.4700000000000002</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>1945</v>
+      </c>
+      <c r="B52">
+        <v>237.6</v>
+      </c>
+      <c r="C52">
+        <v>2.4700000000000002</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>2000</v>
+      </c>
+      <c r="B53">
+        <v>237.6</v>
+      </c>
+      <c r="C53">
+        <v>2.4700000000000002</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>